<commit_message>
Add describe to podkupowacz
</commit_message>
<xml_diff>
--- a/Ikariam/Podkupowacz/Podkupowacze_1.xlsx
+++ b/Ikariam/Podkupowacz/Podkupowacze_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="6675"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="237">
   <si>
     <t>Agusia001</t>
   </si>
@@ -727,6 +727,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>4;34</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1042,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1484,7 +1487,7 @@
         <v>89</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>236</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>91</v>
@@ -2221,7 +2224,6 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
       <c r="E59" s="1" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
Add function to update database
</commit_message>
<xml_diff>
--- a/Ikariam/Podkupowacz/Podkupowacze_1.xlsx
+++ b/Ikariam/Podkupowacz/Podkupowacze_1.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="6675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="237">
   <si>
     <t>Agusia001</t>
   </si>
@@ -186,6 +186,9 @@
     <t>Generat</t>
   </si>
   <si>
+    <t>8;60</t>
+  </si>
+  <si>
     <t>Kosa</t>
   </si>
   <si>
@@ -726,10 +729,7 @@
     <t>9maj</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>4;34</t>
+    <t>Hook</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1042,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1058,25 +1058,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1304,27 +1304,27 @@
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>189</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>28</v>
@@ -1333,44 +1333,44 @@
         <v>29</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -1384,33 +1384,33 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
@@ -1424,13 +1424,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
@@ -1444,93 +1444,93 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>236</v>
+        <v>91</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1544,73 +1544,73 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
@@ -1624,99 +1624,99 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>28</v>
@@ -1742,141 +1742,141 @@
         <v>29</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F39" s="4">
         <v>445</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F40" s="4">
         <v>400</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>14</v>
@@ -1890,53 +1890,53 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>39</v>
@@ -1950,154 +1950,147 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="G49" t="str">
-        <f>B49</f>
-        <v>81;9</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F51" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>28</v>
@@ -2106,24 +2099,24 @@
         <v>29</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
@@ -2137,33 +2130,33 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>14</v>
@@ -2177,171 +2170,181 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>188</v>
+      </c>
       <c r="E57" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E58" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
       <c r="E59" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E60" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E61" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E62" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E63" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E64" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E65" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E66" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E67" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E68" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E69" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>